<commit_message>
se cierra la version 3.5 con el modelo entrenado pero no se logra los resultados esperados, se trabajara con la mas estable 3.3.1
</commit_message>
<xml_diff>
--- a/data/igp/landing/igp-datos-sismicos.xlsx
+++ b/data/igp/landing/igp-datos-sismicos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>fecha UTC</t>
   </si>
@@ -31,145 +31,103 @@
     <t>magnitud (M)</t>
   </si>
   <si>
-    <t>2025-12-01</t>
-  </si>
-  <si>
-    <t>06:36:54</t>
-  </si>
-  <si>
-    <t>-6</t>
-  </si>
-  <si>
-    <t>-81.23</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>2025-12-02</t>
+  </si>
+  <si>
+    <t>01:46:26</t>
+  </si>
+  <si>
+    <t>-6.37</t>
+  </si>
+  <si>
+    <t>-79.49</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>16:41:41</t>
+  </si>
+  <si>
+    <t>-12.4</t>
+  </si>
+  <si>
+    <t>-77.52</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>22:06:45</t>
+  </si>
+  <si>
+    <t>-11.57</t>
+  </si>
+  <si>
+    <t>-77.39</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
+    <t>2025-12-03</t>
+  </si>
+  <si>
+    <t>00:19:45</t>
+  </si>
+  <si>
+    <t>-11.74</t>
+  </si>
+  <si>
+    <t>-76.62</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>2025-12-04</t>
+  </si>
+  <si>
+    <t>07:36:11</t>
+  </si>
+  <si>
+    <t>-8.45</t>
+  </si>
+  <si>
+    <t>-79.7</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>11:15:09</t>
+  </si>
+  <si>
+    <t>-18.6</t>
+  </si>
+  <si>
+    <t>-71.22</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
   <si>
     <t>4.2</t>
-  </si>
-  <si>
-    <t>23:26:59</t>
-  </si>
-  <si>
-    <t>-9.56</t>
-  </si>
-  <si>
-    <t>-75.3</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>23:39:49</t>
-  </si>
-  <si>
-    <t>-14.07</t>
-  </si>
-  <si>
-    <t>-75.9</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>2025-12-02</t>
-  </si>
-  <si>
-    <t>01:46:26</t>
-  </si>
-  <si>
-    <t>-6.37</t>
-  </si>
-  <si>
-    <t>-79.49</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
-    <t>16:41:41</t>
-  </si>
-  <si>
-    <t>-12.4</t>
-  </si>
-  <si>
-    <t>-77.52</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>22:06:45</t>
-  </si>
-  <si>
-    <t>-11.57</t>
-  </si>
-  <si>
-    <t>-77.39</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>4.9</t>
-  </si>
-  <si>
-    <t>2025-12-03</t>
-  </si>
-  <si>
-    <t>00:19:45</t>
-  </si>
-  <si>
-    <t>-11.74</t>
-  </si>
-  <si>
-    <t>-76.62</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>2025-12-04</t>
-  </si>
-  <si>
-    <t>07:36:11</t>
-  </si>
-  <si>
-    <t>-8.45</t>
-  </si>
-  <si>
-    <t>-79.7</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>11:15:09</t>
-  </si>
-  <si>
-    <t>-18.6</t>
-  </si>
-  <si>
-    <t>-71.22</t>
-  </si>
-  <si>
-    <t>16</t>
   </si>
   <si>
     <t>16:34:51</t>
@@ -558,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,47 +621,47 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -718,67 +676,7 @@
         <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version final de la aplicacion lista para productivizar en una primera interface con cron automatico de ETL y predicciones
</commit_message>
<xml_diff>
--- a/data/igp/landing/igp-datos-sismicos.xlsx
+++ b/data/igp/landing/igp-datos-sismicos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>fecha UTC</t>
   </si>
@@ -31,115 +31,133 @@
     <t>magnitud (M)</t>
   </si>
   <si>
-    <t>2025-12-02</t>
-  </si>
-  <si>
-    <t>01:46:26</t>
-  </si>
-  <si>
-    <t>-6.37</t>
-  </si>
-  <si>
-    <t>-79.49</t>
+    <t>2025-12-06</t>
+  </si>
+  <si>
+    <t>16:57:03</t>
+  </si>
+  <si>
+    <t>-8.16</t>
+  </si>
+  <si>
+    <t>-77.18</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>21:40:32</t>
+  </si>
+  <si>
+    <t>-12.03</t>
+  </si>
+  <si>
+    <t>-77.25</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t>3.8</t>
-  </si>
-  <si>
-    <t>16:41:41</t>
-  </si>
-  <si>
-    <t>-12.4</t>
-  </si>
-  <si>
-    <t>-77.52</t>
-  </si>
-  <si>
-    <t>44</t>
+    <t>2025-12-07</t>
+  </si>
+  <si>
+    <t>15:44:02</t>
+  </si>
+  <si>
+    <t>-18.41</t>
+  </si>
+  <si>
+    <t>-70.99</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>23:14:14</t>
+  </si>
+  <si>
+    <t>-17.87</t>
+  </si>
+  <si>
+    <t>-70.03</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
   <si>
     <t>4.6</t>
   </si>
   <si>
-    <t>22:06:45</t>
-  </si>
-  <si>
-    <t>-11.57</t>
-  </si>
-  <si>
-    <t>-77.39</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>4.9</t>
-  </si>
-  <si>
-    <t>2025-12-03</t>
-  </si>
-  <si>
-    <t>00:19:45</t>
-  </si>
-  <si>
-    <t>-11.74</t>
-  </si>
-  <si>
-    <t>-76.62</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>2025-12-04</t>
-  </si>
-  <si>
-    <t>07:36:11</t>
-  </si>
-  <si>
-    <t>-8.45</t>
-  </si>
-  <si>
-    <t>-79.7</t>
+    <t>23:49:15</t>
+  </si>
+  <si>
+    <t>-17.51</t>
+  </si>
+  <si>
+    <t>-70.41</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>2025-12-09</t>
+  </si>
+  <si>
+    <t>00:13:21</t>
+  </si>
+  <si>
+    <t>-6.01</t>
+  </si>
+  <si>
+    <t>-79.91</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>02:46:54</t>
+  </si>
+  <si>
+    <t>-7.25</t>
+  </si>
+  <si>
+    <t>-80.28</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>11:15:09</t>
-  </si>
-  <si>
-    <t>-18.6</t>
-  </si>
-  <si>
-    <t>-71.22</t>
+    <t>04:34:19</t>
+  </si>
+  <si>
+    <t>-15.98</t>
+  </si>
+  <si>
+    <t>-74.89</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>18:56:00</t>
+  </si>
+  <si>
+    <t>-10.68</t>
+  </si>
+  <si>
+    <t>-74.68</t>
   </si>
   <si>
     <t>16</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>16:34:51</t>
-  </si>
-  <si>
-    <t>-15.96</t>
-  </si>
-  <si>
-    <t>-74.18</t>
-  </si>
-  <si>
-    <t>41</t>
   </si>
 </sst>
 </file>
@@ -516,7 +534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,12 +594,12 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -601,82 +619,122 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>11</v>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version mejorada de la landing con popup informativo inicial
</commit_message>
<xml_diff>
--- a/data/igp/landing/igp-datos-sismicos.xlsx
+++ b/data/igp/landing/igp-datos-sismicos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>fecha UTC</t>
   </si>
@@ -29,36 +29,6 @@
   </si>
   <si>
     <t>magnitud (M)</t>
-  </si>
-  <si>
-    <t>2025-12-06</t>
-  </si>
-  <si>
-    <t>16:57:03</t>
-  </si>
-  <si>
-    <t>-8.16</t>
-  </si>
-  <si>
-    <t>-77.18</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>21:40:32</t>
-  </si>
-  <si>
-    <t>-12.03</t>
-  </si>
-  <si>
-    <t>-77.25</t>
-  </si>
-  <si>
-    <t>71</t>
   </si>
   <si>
     <t>2025-12-07</t>
@@ -534,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,12 +564,12 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -614,12 +584,12 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -639,7 +609,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -654,87 +624,47 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version afinada de dashboard
</commit_message>
<xml_diff>
--- a/data/igp/landing/igp-datos-sismicos.xlsx
+++ b/data/igp/landing/igp-datos-sismicos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>fecha UTC</t>
   </si>
@@ -31,81 +31,39 @@
     <t>magnitud (M)</t>
   </si>
   <si>
-    <t>2025-12-07</t>
-  </si>
-  <si>
-    <t>15:44:02</t>
-  </si>
-  <si>
-    <t>-18.41</t>
-  </si>
-  <si>
-    <t>-70.99</t>
-  </si>
-  <si>
-    <t>30</t>
+    <t>2025-12-09</t>
+  </si>
+  <si>
+    <t>00:13:21</t>
+  </si>
+  <si>
+    <t>-6.01</t>
+  </si>
+  <si>
+    <t>-79.91</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>02:46:54</t>
+  </si>
+  <si>
+    <t>-7.25</t>
+  </si>
+  <si>
+    <t>-80.28</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>23:14:14</t>
-  </si>
-  <si>
-    <t>-17.87</t>
-  </si>
-  <si>
-    <t>-70.03</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>23:49:15</t>
-  </si>
-  <si>
-    <t>-17.51</t>
-  </si>
-  <si>
-    <t>-70.41</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>2025-12-09</t>
-  </si>
-  <si>
-    <t>00:13:21</t>
-  </si>
-  <si>
-    <t>-6.01</t>
-  </si>
-  <si>
-    <t>-79.91</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>02:46:54</t>
-  </si>
-  <si>
-    <t>-7.25</t>
-  </si>
-  <si>
-    <t>-80.28</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>04:34:19</t>
   </si>
   <si>
@@ -128,6 +86,39 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>2025-12-10</t>
+  </si>
+  <si>
+    <t>09:23:37</t>
+  </si>
+  <si>
+    <t>-12.03</t>
+  </si>
+  <si>
+    <t>-77.47</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>2025-12-11</t>
+  </si>
+  <si>
+    <t>19:59:41</t>
+  </si>
+  <si>
+    <t>-13.61</t>
+  </si>
+  <si>
+    <t>-72.15</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>3.5</t>
   </si>
 </sst>
 </file>
@@ -504,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -581,47 +572,47 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -629,7 +620,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -641,30 +632,10 @@
         <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>